<commit_message>
Finish login_test without a assertion for the success of authentication
</commit_message>
<xml_diff>
--- a/login_test/teachers.xlsx
+++ b/login_test/teachers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>李雪君</t>
   </si>
@@ -187,6 +187,10 @@
   </si>
   <si>
     <t>Phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -267,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -276,6 +280,9 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -620,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -631,9 +638,10 @@
     <col min="1" max="1" width="19.75" customWidth="1"/>
     <col min="2" max="2" width="19.25" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="26.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>52</v>
       </c>
@@ -643,8 +651,11 @@
       <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D1" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -654,8 +665,11 @@
       <c r="C2" s="1">
         <v>13777277768</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D2" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -665,8 +679,11 @@
       <c r="C3" s="1">
         <v>15268429692</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D3" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -676,8 +693,11 @@
       <c r="C4" s="1">
         <v>13646639945</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D4" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -687,8 +707,11 @@
       <c r="C5" s="1">
         <v>15968443166</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D5" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -698,8 +721,11 @@
       <c r="C6" s="1">
         <v>15957488672</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D6" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -709,8 +735,11 @@
       <c r="C7" s="1">
         <v>15869313633</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D7" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -720,8 +749,11 @@
       <c r="C8" s="1">
         <v>13586875332</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D8" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -731,8 +763,11 @@
       <c r="C9" s="1">
         <v>13586864326</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D9" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -742,8 +777,11 @@
       <c r="C10" s="1">
         <v>13282266511</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D10" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -753,8 +791,11 @@
       <c r="C11" s="1">
         <v>13777230693</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D11" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -764,8 +805,11 @@
       <c r="C12" s="1">
         <v>15867447188</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D12" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -775,8 +819,11 @@
       <c r="C13" s="1">
         <v>13819842828</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D13" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -786,8 +833,11 @@
       <c r="C14" s="1">
         <v>15990253235</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D14" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -797,8 +847,11 @@
       <c r="C15" s="1">
         <v>13858281398</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D15" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -808,8 +861,11 @@
       <c r="C16" s="1">
         <v>15158318899</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D16" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -819,8 +875,11 @@
       <c r="C17" s="1">
         <v>13736131959</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D17" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -830,8 +889,11 @@
       <c r="C18" s="1">
         <v>13586861200</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D18" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -841,8 +903,11 @@
       <c r="C19" s="1">
         <v>13858365778</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D19" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -852,8 +917,11 @@
       <c r="C20" s="1">
         <v>13586873048</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D20" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -863,8 +931,11 @@
       <c r="C21" s="1">
         <v>13626806146</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D21" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -874,8 +945,11 @@
       <c r="C22" s="1">
         <v>13586869788</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D22" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>46</v>
       </c>
@@ -885,8 +959,11 @@
       <c r="C23" s="1">
         <v>13515880608</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D23" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -896,8 +973,11 @@
       <c r="C24" s="1">
         <v>13780050340</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D24" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -907,8 +987,11 @@
       <c r="C25" s="1">
         <v>13606847608</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D25" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -918,8 +1001,11 @@
       <c r="C26" s="1">
         <v>13857460408</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="D26" s="4">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -928,6 +1014,9 @@
       </c>
       <c r="C27" s="1">
         <v>13586871710</v>
+      </c>
+      <c r="D27" s="4">
+        <v>111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>